<commit_message>
Funciones parte 1 corregidas
</commit_message>
<xml_diff>
--- a/files/History5400732.xlsx
+++ b/files/History5400732.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AnapauGiusti/Documents/Microestructuras y Sistemas de Trading/MyST_LAB_3_E3/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD413CBA-F8C3-9F4A-A855-3914E6EC4125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E98C2A19-CDAF-8E49-AD2E-785BB0C03F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{C08C49E9-9083-C745-AE38-6174E27D12B8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
   <si>
     <t>Time</t>
   </si>
@@ -313,9 +313,6 @@
   </si>
   <si>
     <t>opentime</t>
-  </si>
-  <si>
-    <t>type</t>
   </si>
   <si>
     <t>OpenTime</t>
@@ -709,225 +706,243 @@
   <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>45426490</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>1.3648199999999999</v>
+      </c>
+      <c r="H2">
+        <v>1.3419099999999999</v>
+      </c>
+      <c r="I2">
+        <v>1.4169099999999999</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>1.36541</v>
+      </c>
+      <c r="L2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>45448836</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3">
+        <v>1.1722399999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.17272</v>
+      </c>
+      <c r="I3">
+        <v>1.17072</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>1.1727099999999999</v>
+      </c>
+      <c r="L3">
+        <v>-4.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>45426490</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>45470330</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.72540000000000004</v>
+      </c>
+      <c r="H4">
+        <v>0.73067000000000004</v>
+      </c>
+      <c r="I4">
+        <v>0.71567000000000003</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>0.73067000000000004</v>
+      </c>
+      <c r="L4">
+        <v>-105.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>45498648</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0.1</v>
       </c>
-      <c r="F2">
-        <v>1.3648199999999999</v>
-      </c>
-      <c r="G2">
-        <v>1.3419099999999999</v>
-      </c>
-      <c r="H2">
-        <v>1.4169099999999999</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>1.36541</v>
-      </c>
-      <c r="K2">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>45448836</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="G5">
+        <v>1.2654799999999999</v>
+      </c>
+      <c r="H5">
+        <v>1.2606200000000001</v>
+      </c>
+      <c r="I5">
+        <v>1.27189</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <v>1.2669900000000001</v>
+      </c>
+      <c r="L5">
+        <v>11.92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>45522977</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>0.1</v>
       </c>
-      <c r="F3">
-        <v>1.1722399999999999</v>
-      </c>
-      <c r="G3">
-        <v>1.17272</v>
-      </c>
-      <c r="H3">
-        <v>1.17072</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3">
-        <v>1.1727099999999999</v>
-      </c>
-      <c r="K3">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>45470330</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>0.2</v>
-      </c>
-      <c r="F4">
-        <v>0.72540000000000004</v>
-      </c>
-      <c r="G4">
-        <v>0.73067000000000004</v>
-      </c>
-      <c r="H4">
-        <v>0.71567000000000003</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <v>0.73067000000000004</v>
-      </c>
-      <c r="K4">
-        <v>-105.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5">
-        <v>45498648</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0.1</v>
-      </c>
-      <c r="F5">
-        <v>1.2654799999999999</v>
-      </c>
-      <c r="G5">
-        <v>1.2606200000000001</v>
-      </c>
-      <c r="H5">
-        <v>1.27189</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5">
-        <v>1.2669900000000001</v>
-      </c>
-      <c r="K5">
-        <v>11.92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6">
-        <v>45522977</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0.1</v>
-      </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.70233999999999996</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.70023999999999997</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>70507</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>26</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.70009999999999994</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>-22.4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>

</xml_diff>